<commit_message>
al ost finished clustering writeup
</commit_message>
<xml_diff>
--- a/JournalPaper/Tables/RulesTable.xlsx
+++ b/JournalPaper/Tables/RulesTable.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="129">
   <si>
     <t>ID</t>
   </si>
@@ -85,9 +85,6 @@
     <t>P10</t>
   </si>
   <si>
-    <t>P11</t>
-  </si>
-  <si>
     <t>Rules</t>
   </si>
   <si>
@@ -271,12 +268,6 @@
     <t>T10</t>
   </si>
   <si>
-    <t>P4###</t>
-  </si>
-  <si>
-    <t>P5###</t>
-  </si>
-  <si>
     <t>P6</t>
   </si>
   <si>
@@ -349,9 +340,6 @@
     <t>E6</t>
   </si>
   <si>
-    <t>100 mBar</t>
-  </si>
-  <si>
     <t>E7</t>
   </si>
   <si>
@@ -362,19 +350,195 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>Compressor power</t>
+  </si>
+  <si>
+    <t>K3</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">25 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>°C</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">140 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>°C</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">22 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>°C</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">100 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>°C</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">21 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>°C</t>
+    </r>
+  </si>
+  <si>
+    <t>2.5 barg</t>
+  </si>
+  <si>
+    <t>7.250 barg</t>
+  </si>
+  <si>
+    <t>7.25 barg</t>
+  </si>
+  <si>
+    <t>1.5 kW</t>
+  </si>
+  <si>
+    <t>8.4 kW</t>
+  </si>
+  <si>
+    <r>
+      <t>35</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>°C</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">155 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>°C</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">24 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>°C</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">120 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>°C</t>
+    </r>
+  </si>
+  <si>
+    <t>2.6 barg</t>
+  </si>
+  <si>
+    <t>7.6 barg</t>
+  </si>
+  <si>
+    <t>0.1 barg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -397,12 +561,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,18 +889,18 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
       <c r="AA3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AB3" s="2"/>
     </row>
     <row r="4" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>9</v>
@@ -762,34 +930,34 @@
         <v>18</v>
       </c>
       <c r="N4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="S4" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="T4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="V4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="W4" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="AA4" t="s">
         <v>0</v>
@@ -803,25 +971,25 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA5">
         <v>1</v>
       </c>
       <c r="AB5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="4:28" x14ac:dyDescent="0.25">
@@ -829,25 +997,25 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA6">
         <v>2</v>
       </c>
       <c r="AB6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="4:28" x14ac:dyDescent="0.25">
@@ -855,25 +1023,25 @@
         <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA7">
         <v>3</v>
       </c>
       <c r="AB7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="4:28" x14ac:dyDescent="0.25">
@@ -881,22 +1049,22 @@
         <v>4</v>
       </c>
       <c r="H8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA8">
         <v>4</v>
       </c>
       <c r="AB8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="4:28" x14ac:dyDescent="0.25">
@@ -904,16 +1072,16 @@
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA9">
         <v>5</v>
       </c>
       <c r="AB9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="4:28" x14ac:dyDescent="0.25">
@@ -921,22 +1089,22 @@
         <v>6</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA10">
         <v>6</v>
       </c>
       <c r="AB10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="4:28" x14ac:dyDescent="0.25">
@@ -944,22 +1112,22 @@
         <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA11">
         <v>7</v>
       </c>
       <c r="AB11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="4:28" x14ac:dyDescent="0.25">
@@ -967,22 +1135,22 @@
         <v>8</v>
       </c>
       <c r="H12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA12">
         <v>8</v>
       </c>
       <c r="AB12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="4:28" x14ac:dyDescent="0.25">
@@ -990,22 +1158,22 @@
         <v>9</v>
       </c>
       <c r="I13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA13">
         <v>9</v>
       </c>
       <c r="AB13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="4:28" x14ac:dyDescent="0.25">
@@ -1013,13 +1181,13 @@
         <v>10</v>
       </c>
       <c r="J14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA14">
         <v>10</v>
@@ -1033,16 +1201,16 @@
         <v>11</v>
       </c>
       <c r="K15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA15">
         <v>11</v>
@@ -1056,16 +1224,16 @@
         <v>12</v>
       </c>
       <c r="L16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA16">
         <v>12</v>
@@ -1079,13 +1247,13 @@
         <v>13</v>
       </c>
       <c r="M17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA17">
         <v>13</v>
@@ -1099,16 +1267,16 @@
         <v>14</v>
       </c>
       <c r="F18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA18">
         <v>14</v>
@@ -1122,16 +1290,16 @@
         <v>15</v>
       </c>
       <c r="H19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA19">
         <v>15</v>
@@ -1166,7 +1334,7 @@
   <sheetData>
     <row r="3" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
@@ -1177,7 +1345,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="4:5" x14ac:dyDescent="0.25">
@@ -1185,7 +1353,7 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="4:5" x14ac:dyDescent="0.25">
@@ -1193,7 +1361,7 @@
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="4:5" x14ac:dyDescent="0.25">
@@ -1201,7 +1369,7 @@
         <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="4:5" x14ac:dyDescent="0.25">
@@ -1209,7 +1377,7 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="4:5" x14ac:dyDescent="0.25">
@@ -1217,7 +1385,7 @@
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="4:5" x14ac:dyDescent="0.25">
@@ -1225,7 +1393,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="4:5" x14ac:dyDescent="0.25">
@@ -1233,7 +1401,7 @@
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1243,10 +1411,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:E55"/>
+  <dimension ref="C3:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:E55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E56" sqref="C3:E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,32 +1424,32 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" t="s">
-        <v>75</v>
+      <c r="E3" s="4" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C4" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="C4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.25">
@@ -1289,10 +1457,10 @@
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.25">
@@ -1300,10 +1468,10 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.25">
@@ -1311,10 +1479,10 @@
         <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
@@ -1322,10 +1490,10 @@
         <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.25">
@@ -1333,10 +1501,10 @@
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E10" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
@@ -1344,10 +1512,10 @@
         <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.25">
@@ -1355,476 +1523,484 @@
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>17</v>
+        <v>108</v>
       </c>
       <c r="D13" t="s">
         <v>48</v>
       </c>
       <c r="E13" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>18</v>
+        <v>109</v>
       </c>
       <c r="D14" t="s">
         <v>49</v>
       </c>
       <c r="E14" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="C16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" t="s">
-        <v>111</v>
-      </c>
+      <c r="C17" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E18" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E19" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E20" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E21" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E22" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E23" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+      <c r="C24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>76</v>
-      </c>
-      <c r="D25" t="s">
-        <v>40</v>
-      </c>
-      <c r="E25">
-        <v>25</v>
-      </c>
+      <c r="C25" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D26" t="s">
-        <v>41</v>
-      </c>
-      <c r="E26">
-        <v>140</v>
+        <v>39</v>
+      </c>
+      <c r="E26" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D27" t="s">
-        <v>42</v>
-      </c>
-      <c r="E27">
-        <v>22</v>
+        <v>40</v>
+      </c>
+      <c r="E27" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D28" t="s">
-        <v>43</v>
-      </c>
-      <c r="E28">
-        <v>100</v>
+        <v>41</v>
+      </c>
+      <c r="E28" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D29" t="s">
-        <v>44</v>
-      </c>
-      <c r="E29">
-        <v>21</v>
+        <v>42</v>
+      </c>
+      <c r="E29" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D30" t="s">
-        <v>45</v>
-      </c>
-      <c r="E30">
-        <v>2500</v>
+        <v>43</v>
+      </c>
+      <c r="E30" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D31" t="s">
-        <v>46</v>
-      </c>
-      <c r="E31">
-        <v>7250</v>
+        <v>44</v>
+      </c>
+      <c r="E31" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="D32" t="s">
-        <v>47</v>
-      </c>
-      <c r="E32">
-        <v>7250</v>
+        <v>45</v>
+      </c>
+      <c r="E32" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="D33" t="s">
-        <v>48</v>
-      </c>
-      <c r="E33">
-        <v>1</v>
+        <v>46</v>
+      </c>
+      <c r="E33" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D34" t="s">
-        <v>86</v>
+        <v>47</v>
       </c>
       <c r="E34">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D35" t="s">
-        <v>88</v>
-      </c>
-      <c r="E35">
-        <v>8.4</v>
+        <v>83</v>
+      </c>
+      <c r="E35" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C36" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
+      <c r="C36" t="s">
+        <v>111</v>
+      </c>
+      <c r="D36" t="s">
+        <v>85</v>
+      </c>
+      <c r="E36" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>90</v>
-      </c>
-      <c r="D37" t="s">
-        <v>40</v>
-      </c>
-      <c r="E37">
-        <v>35</v>
-      </c>
+      <c r="C37" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D38" t="s">
-        <v>41</v>
-      </c>
-      <c r="E38">
-        <v>155</v>
+        <v>39</v>
+      </c>
+      <c r="E38" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D39" t="s">
-        <v>42</v>
-      </c>
-      <c r="E39">
-        <v>24</v>
+        <v>40</v>
+      </c>
+      <c r="E39" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D40" t="s">
-        <v>43</v>
-      </c>
-      <c r="E40">
-        <v>120</v>
+        <v>41</v>
+      </c>
+      <c r="E40" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D41" t="s">
-        <v>44</v>
-      </c>
-      <c r="E41">
-        <v>21</v>
+        <v>42</v>
+      </c>
+      <c r="E41" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D42" t="s">
-        <v>45</v>
-      </c>
-      <c r="E42">
-        <v>2600</v>
+        <v>43</v>
+      </c>
+      <c r="E42" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D43" t="s">
-        <v>46</v>
-      </c>
-      <c r="E43">
-        <v>7510</v>
+        <v>44</v>
+      </c>
+      <c r="E43" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="44" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D44" t="s">
-        <v>47</v>
-      </c>
-      <c r="E44">
-        <v>7510</v>
+        <v>45</v>
+      </c>
+      <c r="E44" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D45" t="s">
-        <v>48</v>
-      </c>
-      <c r="E45">
+        <v>46</v>
+      </c>
+      <c r="E45" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>95</v>
+      </c>
+      <c r="D46" t="s">
+        <v>47</v>
+      </c>
+      <c r="E46">
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C46" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-    </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
-        <v>100</v>
-      </c>
-      <c r="D47" t="s">
-        <v>40</v>
-      </c>
-      <c r="E47" t="s">
-        <v>101</v>
-      </c>
+      <c r="C47" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
     </row>
     <row r="48" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D48" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E48" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D49" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E49" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E50" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D51" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E51" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="52" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D52" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E52" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D53" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E53" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
     </row>
     <row r="54" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D54" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E54" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
     </row>
     <row r="55" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D55" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E55" t="s">
-        <v>107</v>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>106</v>
+      </c>
+      <c r="D56" t="s">
+        <v>48</v>
+      </c>
+      <c r="E56" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C47:E47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
finished draft a of journal paper
</commit_message>
<xml_diff>
--- a/JournalPaper/Tables/RulesTable.xlsx
+++ b/JournalPaper/Tables/RulesTable.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11685" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11685" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
-    <sheet name="Modes" sheetId="3" r:id="rId2"/>
-    <sheet name="Naming Convention" sheetId="2" r:id="rId3"/>
+    <sheet name="RuleImpact" sheetId="5" r:id="rId2"/>
+    <sheet name="Modes" sheetId="3" r:id="rId3"/>
+    <sheet name="Naming Convention" sheetId="2" r:id="rId4"/>
+    <sheet name="ModeApplication" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="131">
   <si>
     <t>ID</t>
   </si>
@@ -512,6 +514,12 @@
   </si>
   <si>
     <t>0.1 barg</t>
+  </si>
+  <si>
+    <t>3:8</t>
+  </si>
+  <si>
+    <t>RuleImpact</t>
   </si>
 </sst>
 </file>
@@ -561,16 +569,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -854,7 +863,7 @@
   <dimension ref="D3:AB19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:W19"/>
+      <selection activeCell="U3" sqref="U3:W19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,33 +879,33 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2" t="s">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="AA3" s="2" t="s">
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="AA3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AB3" s="2"/>
+      <c r="AB3" s="3"/>
     </row>
     <row r="4" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
@@ -1320,6 +1329,203 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>15</v>
+      </c>
+      <c r="D19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C3:E3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:E11"/>
   <sheetViews>
@@ -1409,11 +1615,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E56" sqref="C3:E56"/>
     </sheetView>
   </sheetViews>
@@ -1424,22 +1630,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
@@ -1571,11 +1777,11 @@
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
@@ -1655,11 +1861,11 @@
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
@@ -1783,11 +1989,11 @@
       </c>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
@@ -1889,11 +2095,11 @@
       </c>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
     </row>
     <row r="48" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
@@ -2005,4 +2211,446 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:L18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <v>6</v>
+      </c>
+      <c r="K3">
+        <v>7</v>
+      </c>
+      <c r="L3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" t="s">
+        <v>26</v>
+      </c>
+      <c r="L11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K12" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" t="s">
+        <v>26</v>
+      </c>
+      <c r="L13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" t="s">
+        <v>26</v>
+      </c>
+      <c r="K15" t="s">
+        <v>26</v>
+      </c>
+      <c r="L15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I16" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K16" t="s">
+        <v>26</v>
+      </c>
+      <c r="L16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>14</v>
+      </c>
+      <c r="F17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I17" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" t="s">
+        <v>26</v>
+      </c>
+      <c r="K17" t="s">
+        <v>26</v>
+      </c>
+      <c r="L17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>15</v>
+      </c>
+      <c r="F18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" t="s">
+        <v>26</v>
+      </c>
+      <c r="K18" t="s">
+        <v>26</v>
+      </c>
+      <c r="L18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D2:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finished bar the shouting
</commit_message>
<xml_diff>
--- a/JournalPaper/Tables/RulesTable.xlsx
+++ b/JournalPaper/Tables/RulesTable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11685" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11685" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="132">
   <si>
     <t>ID</t>
   </si>
@@ -520,6 +520,9 @@
   </si>
   <si>
     <t>RuleImpact</t>
+  </si>
+  <si>
+    <t>CAGI Input Power (kW)</t>
   </si>
 </sst>
 </file>
@@ -569,17 +572,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -860,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:AB19"/>
+  <dimension ref="D3:AC19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U3" sqref="U3:W19"/>
+      <selection activeCell="U3" sqref="U3:X19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,39 +881,41 @@
     <col min="12" max="12" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="20" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.140625" customWidth="1"/>
+    <col min="22" max="24" width="3.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="E3" s="3" t="s">
+    <row r="3" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="E3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3" t="s">
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="AA3" s="3" t="s">
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="AB3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="AB3" s="3"/>
-    </row>
-    <row r="4" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="AC3" s="5"/>
+    </row>
+    <row r="4" spans="4:29" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>61</v>
       </c>
@@ -959,23 +967,26 @@
       <c r="T4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="U4" t="s">
+        <v>61</v>
+      </c>
+      <c r="V4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="W4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="X4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>0</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="4:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:29" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>1</v>
       </c>
@@ -988,20 +999,23 @@
       <c r="N5" t="s">
         <v>26</v>
       </c>
-      <c r="U5" t="s">
-        <v>26</v>
-      </c>
-      <c r="W5" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA5">
+      <c r="U5">
         <v>1</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="V5" t="s">
+        <v>26</v>
+      </c>
+      <c r="X5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB5">
+        <v>1</v>
+      </c>
+      <c r="AC5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="4:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:29" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>2</v>
       </c>
@@ -1014,20 +1028,23 @@
       <c r="O6" t="s">
         <v>26</v>
       </c>
-      <c r="V6" t="s">
-        <v>26</v>
+      <c r="U6">
+        <v>2</v>
       </c>
       <c r="W6" t="s">
         <v>26</v>
       </c>
-      <c r="AA6">
+      <c r="X6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB6">
         <v>2</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="4:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:29" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>3</v>
       </c>
@@ -1040,20 +1057,23 @@
       <c r="P7" t="s">
         <v>26</v>
       </c>
-      <c r="U7" t="s">
-        <v>26</v>
-      </c>
-      <c r="W7" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA7">
+      <c r="U7">
         <v>3</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="V7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X7" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB7">
+        <v>3</v>
+      </c>
+      <c r="AC7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="4:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:29" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>4</v>
       </c>
@@ -1066,34 +1086,40 @@
       <c r="Q8" t="s">
         <v>26</v>
       </c>
-      <c r="V8" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA8">
+      <c r="U8">
         <v>4</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="W8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB8">
+        <v>4</v>
+      </c>
+      <c r="AC8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="4:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:29" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>5</v>
       </c>
       <c r="E9" t="s">
         <v>26</v>
       </c>
-      <c r="V9" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA9">
+      <c r="U9">
         <v>5</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="W9" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB9">
+        <v>5</v>
+      </c>
+      <c r="AC9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="4:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:29" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>6</v>
       </c>
@@ -1103,20 +1129,23 @@
       <c r="N10" t="s">
         <v>26</v>
       </c>
-      <c r="V10" t="s">
-        <v>26</v>
+      <c r="U10">
+        <v>6</v>
       </c>
       <c r="W10" t="s">
         <v>26</v>
       </c>
-      <c r="AA10">
+      <c r="X10" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB10">
         <v>6</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AC10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="4:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:29" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>7</v>
       </c>
@@ -1126,20 +1155,23 @@
       <c r="O11" t="s">
         <v>26</v>
       </c>
-      <c r="V11" t="s">
-        <v>26</v>
+      <c r="U11">
+        <v>7</v>
       </c>
       <c r="W11" t="s">
         <v>26</v>
       </c>
-      <c r="AA11">
+      <c r="X11" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB11">
         <v>7</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AC11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="4:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:29" x14ac:dyDescent="0.25">
       <c r="D12">
         <v>8</v>
       </c>
@@ -1149,20 +1181,23 @@
       <c r="P12" t="s">
         <v>26</v>
       </c>
-      <c r="V12" t="s">
-        <v>26</v>
+      <c r="U12">
+        <v>8</v>
       </c>
       <c r="W12" t="s">
         <v>26</v>
       </c>
-      <c r="AA12">
+      <c r="X12" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB12">
         <v>8</v>
       </c>
-      <c r="AB12" t="s">
+      <c r="AC12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="4:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:29" x14ac:dyDescent="0.25">
       <c r="D13">
         <v>9</v>
       </c>
@@ -1172,20 +1207,23 @@
       <c r="Q13" t="s">
         <v>26</v>
       </c>
-      <c r="V13" t="s">
-        <v>26</v>
+      <c r="U13">
+        <v>9</v>
       </c>
       <c r="W13" t="s">
         <v>26</v>
       </c>
-      <c r="AA13">
+      <c r="X13" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB13">
         <v>9</v>
       </c>
-      <c r="AB13" t="s">
+      <c r="AC13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="4:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:29" x14ac:dyDescent="0.25">
       <c r="D14">
         <v>10</v>
       </c>
@@ -1195,17 +1233,20 @@
       <c r="N14" t="s">
         <v>26</v>
       </c>
-      <c r="U14" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA14">
+      <c r="U14">
         <v>10</v>
       </c>
-      <c r="AB14" t="s">
+      <c r="V14" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB14">
+        <v>10</v>
+      </c>
+      <c r="AC14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="4:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:29" x14ac:dyDescent="0.25">
       <c r="D15">
         <v>11</v>
       </c>
@@ -1215,20 +1256,23 @@
       <c r="T15" t="s">
         <v>26</v>
       </c>
-      <c r="V15" t="s">
-        <v>26</v>
+      <c r="U15">
+        <v>11</v>
       </c>
       <c r="W15" t="s">
         <v>26</v>
       </c>
-      <c r="AA15">
+      <c r="X15" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB15">
         <v>11</v>
       </c>
-      <c r="AB15" t="s">
+      <c r="AC15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="4:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:29" x14ac:dyDescent="0.25">
       <c r="D16">
         <v>12</v>
       </c>
@@ -1238,20 +1282,23 @@
       <c r="R16" t="s">
         <v>26</v>
       </c>
-      <c r="V16" t="s">
-        <v>26</v>
+      <c r="U16">
+        <v>12</v>
       </c>
       <c r="W16" t="s">
         <v>26</v>
       </c>
-      <c r="AA16">
+      <c r="X16" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB16">
         <v>12</v>
       </c>
-      <c r="AB16" t="s">
+      <c r="AC16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="4:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:29" x14ac:dyDescent="0.25">
       <c r="D17">
         <v>13</v>
       </c>
@@ -1261,17 +1308,20 @@
       <c r="S17" t="s">
         <v>26</v>
       </c>
-      <c r="W17" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA17">
+      <c r="U17">
         <v>13</v>
       </c>
-      <c r="AB17" t="s">
+      <c r="X17" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB17">
+        <v>13</v>
+      </c>
+      <c r="AC17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="4:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:29" x14ac:dyDescent="0.25">
       <c r="D18">
         <v>14</v>
       </c>
@@ -1281,20 +1331,23 @@
       <c r="N18" t="s">
         <v>26</v>
       </c>
-      <c r="V18" t="s">
-        <v>26</v>
+      <c r="U18">
+        <v>14</v>
       </c>
       <c r="W18" t="s">
         <v>26</v>
       </c>
-      <c r="AA18">
+      <c r="X18" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB18">
         <v>14</v>
       </c>
-      <c r="AB18" t="s">
+      <c r="AC18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="4:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:29" x14ac:dyDescent="0.25">
       <c r="D19">
         <v>15</v>
       </c>
@@ -1304,24 +1357,27 @@
       <c r="P19" t="s">
         <v>26</v>
       </c>
-      <c r="V19" t="s">
-        <v>26</v>
+      <c r="U19">
+        <v>15</v>
       </c>
       <c r="W19" t="s">
         <v>26</v>
       </c>
-      <c r="AA19">
+      <c r="X19" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB19">
         <v>15</v>
       </c>
-      <c r="AB19" t="s">
+      <c r="AC19" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="AB3:AC3"/>
     <mergeCell ref="E3:T3"/>
-    <mergeCell ref="U3:W3"/>
+    <mergeCell ref="V3:X3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1332,7 +1388,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3:E19"/>
     </sheetView>
   </sheetViews>
@@ -1344,11 +1400,11 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -1527,10 +1583,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:E11"/>
+  <dimension ref="D3:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:E11"/>
+      <selection activeCell="D3" sqref="D3:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1538,76 +1594,103 @@
     <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>62</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="5" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="6" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>3</v>
       </c>
       <c r="E6" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="7" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>4</v>
       </c>
       <c r="E7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="8" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>27.2</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>5</v>
       </c>
       <c r="E8" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="9" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>31.2</v>
+      </c>
+    </row>
+    <row r="9" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>6</v>
       </c>
       <c r="E9" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="10" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>38.299999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>7</v>
       </c>
       <c r="E10" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="11" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>42.6</v>
+      </c>
+    </row>
+    <row r="11" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>8</v>
       </c>
       <c r="E11" t="s">
         <v>70</v>
+      </c>
+      <c r="F11">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1617,19 +1700,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:E56"/>
+  <dimension ref="C3:O56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E56" sqref="C3:E56"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
         <v>37</v>
       </c>
@@ -1639,15 +1728,53 @@
       <c r="E3" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C4" s="4" t="s">
+      <c r="H3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C4" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="H4" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>9</v>
       </c>
@@ -1657,8 +1784,32 @@
       <c r="E5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" t="s">
+        <v>87</v>
+      </c>
+      <c r="K5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" t="s">
+        <v>122</v>
+      </c>
+      <c r="M5" t="s">
+        <v>75</v>
+      </c>
+      <c r="N5" t="s">
+        <v>39</v>
+      </c>
+      <c r="O5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>10</v>
       </c>
@@ -1668,8 +1819,32 @@
       <c r="E6" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" t="s">
+        <v>88</v>
+      </c>
+      <c r="K6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" t="s">
+        <v>123</v>
+      </c>
+      <c r="M6" t="s">
+        <v>76</v>
+      </c>
+      <c r="N6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>11</v>
       </c>
@@ -1679,8 +1854,32 @@
       <c r="E7" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" t="s">
+        <v>89</v>
+      </c>
+      <c r="K7" t="s">
+        <v>41</v>
+      </c>
+      <c r="L7" t="s">
+        <v>124</v>
+      </c>
+      <c r="M7" t="s">
+        <v>77</v>
+      </c>
+      <c r="N7" t="s">
+        <v>41</v>
+      </c>
+      <c r="O7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>12</v>
       </c>
@@ -1690,8 +1889,32 @@
       <c r="E8" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" t="s">
+        <v>90</v>
+      </c>
+      <c r="K8" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" t="s">
+        <v>125</v>
+      </c>
+      <c r="M8" t="s">
+        <v>78</v>
+      </c>
+      <c r="N8" t="s">
+        <v>42</v>
+      </c>
+      <c r="O8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>13</v>
       </c>
@@ -1701,8 +1924,32 @@
       <c r="E9" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" t="s">
+        <v>91</v>
+      </c>
+      <c r="K9" t="s">
+        <v>43</v>
+      </c>
+      <c r="L9" t="s">
+        <v>116</v>
+      </c>
+      <c r="M9" t="s">
+        <v>79</v>
+      </c>
+      <c r="N9" t="s">
+        <v>43</v>
+      </c>
+      <c r="O9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>14</v>
       </c>
@@ -1712,8 +1959,32 @@
       <c r="E10" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" t="s">
+        <v>92</v>
+      </c>
+      <c r="K10" t="s">
+        <v>44</v>
+      </c>
+      <c r="L10" t="s">
+        <v>126</v>
+      </c>
+      <c r="M10" t="s">
+        <v>80</v>
+      </c>
+      <c r="N10" t="s">
+        <v>44</v>
+      </c>
+      <c r="O10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>15</v>
       </c>
@@ -1723,8 +1994,32 @@
       <c r="E11" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" t="s">
+        <v>45</v>
+      </c>
+      <c r="J11" t="s">
+        <v>93</v>
+      </c>
+      <c r="K11" t="s">
+        <v>45</v>
+      </c>
+      <c r="L11" t="s">
+        <v>127</v>
+      </c>
+      <c r="M11" t="s">
+        <v>92</v>
+      </c>
+      <c r="N11" t="s">
+        <v>45</v>
+      </c>
+      <c r="O11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>16</v>
       </c>
@@ -1734,8 +2029,32 @@
       <c r="E12" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" t="s">
+        <v>94</v>
+      </c>
+      <c r="K12" t="s">
+        <v>46</v>
+      </c>
+      <c r="L12" t="s">
+        <v>127</v>
+      </c>
+      <c r="M12" t="s">
+        <v>93</v>
+      </c>
+      <c r="N12" t="s">
+        <v>46</v>
+      </c>
+      <c r="O12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>108</v>
       </c>
@@ -1745,8 +2064,32 @@
       <c r="E13" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>108</v>
+      </c>
+      <c r="I13" t="s">
+        <v>48</v>
+      </c>
+      <c r="J13" t="s">
+        <v>95</v>
+      </c>
+      <c r="K13" t="s">
+        <v>47</v>
+      </c>
+      <c r="L13">
+        <v>2</v>
+      </c>
+      <c r="M13" t="s">
+        <v>81</v>
+      </c>
+      <c r="N13" t="s">
+        <v>47</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>109</v>
       </c>
@@ -1756,8 +2099,28 @@
       <c r="E14" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>109</v>
+      </c>
+      <c r="I14" t="s">
+        <v>49</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" t="s">
+        <v>84</v>
+      </c>
+      <c r="N14" t="s">
+        <v>83</v>
+      </c>
+      <c r="O14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>17</v>
       </c>
@@ -1767,23 +2130,75 @@
       <c r="E15" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" t="s">
+        <v>47</v>
+      </c>
+      <c r="J15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K15" t="s">
+        <v>39</v>
+      </c>
+      <c r="L15" t="s">
+        <v>98</v>
+      </c>
+      <c r="M15" t="s">
+        <v>111</v>
+      </c>
+      <c r="N15" t="s">
+        <v>85</v>
+      </c>
+      <c r="O15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>82</v>
       </c>
       <c r="D16" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="4" t="s">
+      <c r="H16" t="s">
+        <v>82</v>
+      </c>
+      <c r="I16" t="s">
+        <v>110</v>
+      </c>
+      <c r="J16" t="s">
+        <v>99</v>
+      </c>
+      <c r="K16" t="s">
+        <v>40</v>
+      </c>
+      <c r="L16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C17" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="H17" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="I17" s="6"/>
+      <c r="J17" t="s">
+        <v>100</v>
+      </c>
+      <c r="K17" t="s">
+        <v>41</v>
+      </c>
+      <c r="L17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>20</v>
       </c>
@@ -1793,8 +2208,23 @@
       <c r="E18" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" t="s">
+        <v>50</v>
+      </c>
+      <c r="J18" t="s">
+        <v>101</v>
+      </c>
+      <c r="K18" t="s">
+        <v>42</v>
+      </c>
+      <c r="L18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>21</v>
       </c>
@@ -1804,8 +2234,23 @@
       <c r="E19" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" t="s">
+        <v>51</v>
+      </c>
+      <c r="J19" t="s">
+        <v>102</v>
+      </c>
+      <c r="K19" t="s">
+        <v>43</v>
+      </c>
+      <c r="L19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>22</v>
       </c>
@@ -1815,8 +2260,23 @@
       <c r="E20" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" t="s">
+        <v>52</v>
+      </c>
+      <c r="J20" t="s">
+        <v>103</v>
+      </c>
+      <c r="K20" t="s">
+        <v>44</v>
+      </c>
+      <c r="L20" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>23</v>
       </c>
@@ -1826,8 +2286,23 @@
       <c r="E21" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" t="s">
+        <v>53</v>
+      </c>
+      <c r="J21" t="s">
+        <v>104</v>
+      </c>
+      <c r="K21" t="s">
+        <v>45</v>
+      </c>
+      <c r="L21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>24</v>
       </c>
@@ -1837,8 +2312,23 @@
       <c r="E22" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>24</v>
+      </c>
+      <c r="I22" t="s">
+        <v>54</v>
+      </c>
+      <c r="J22" t="s">
+        <v>105</v>
+      </c>
+      <c r="K22" t="s">
+        <v>46</v>
+      </c>
+      <c r="L22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>25</v>
       </c>
@@ -1848,8 +2338,23 @@
       <c r="E23" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>25</v>
+      </c>
+      <c r="I23" t="s">
+        <v>55</v>
+      </c>
+      <c r="J23" t="s">
+        <v>106</v>
+      </c>
+      <c r="K23" t="s">
+        <v>48</v>
+      </c>
+      <c r="L23" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>27</v>
       </c>
@@ -1859,15 +2364,23 @@
       <c r="E24" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="4" t="s">
+      <c r="H24" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C25" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>75</v>
       </c>
@@ -1878,7 +2391,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>76</v>
       </c>
@@ -1889,7 +2402,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>77</v>
       </c>
@@ -1900,7 +2413,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>78</v>
       </c>
@@ -1911,7 +2424,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>79</v>
       </c>
@@ -1922,7 +2435,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>80</v>
       </c>
@@ -1933,7 +2446,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>92</v>
       </c>
@@ -1989,11 +2502,11 @@
       </c>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
@@ -2095,11 +2608,11 @@
       </c>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
     </row>
     <row r="48" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
@@ -2201,12 +2714,18 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="11">
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="C25:E25"/>
     <mergeCell ref="C37:E37"/>
     <mergeCell ref="C47:E47"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="J14:L14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2217,18 +2736,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -2246,7 +2765,7 @@
       <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="3" t="s">
         <v>129</v>
       </c>
       <c r="G3">

</xml_diff>